<commit_message>
customer login and rating product
</commit_message>
<xml_diff>
--- a/Documents/Requirement Attributes.xlsx
+++ b/Documents/Requirement Attributes.xlsx
@@ -242,9 +242,6 @@
     <t>PRODUCT MODULE</t>
   </si>
   <si>
-    <t>Best selling products</t>
-  </si>
-  <si>
     <t>Related products</t>
   </si>
   <si>
@@ -369,6 +366,9 @@
   </si>
   <si>
     <t>Implemented</t>
+  </si>
+  <si>
+    <t>Best selling/recommended products</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1137,7 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1245,7 +1245,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="F6" s="39" t="s">
         <v>11</v>
@@ -1268,7 +1268,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F7" s="39" t="s">
         <v>11</v>
@@ -1314,7 +1314,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="F9" s="39" t="s">
         <v>11</v>
@@ -1408,7 +1408,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="40" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="F13" s="39" t="s">
         <v>10</v>
@@ -1466,7 +1466,7 @@
         <v>8</v>
       </c>
       <c r="E17" s="47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F17" s="46" t="s">
         <v>11</v>
@@ -1489,7 +1489,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F18" s="46" t="s">
         <v>11</v>
@@ -1535,7 +1535,7 @@
         <v>8</v>
       </c>
       <c r="E20" s="47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F20" s="46" t="s">
         <v>10</v>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="50" t="s">
         <v>50</v>
@@ -1674,7 +1674,7 @@
         <v>8</v>
       </c>
       <c r="E27" s="53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F27" s="52" t="s">
         <v>11</v>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" s="50" t="s">
         <v>51</v>
@@ -1697,7 +1697,7 @@
         <v>8</v>
       </c>
       <c r="E28" s="53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F28" s="52" t="s">
         <v>11</v>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="50" t="s">
         <v>52</v>
@@ -1720,7 +1720,7 @@
         <v>8</v>
       </c>
       <c r="E29" s="53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F29" s="52" t="s">
         <v>11</v>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="50" t="s">
         <v>53</v>
@@ -1743,7 +1743,7 @@
         <v>8</v>
       </c>
       <c r="E30" s="53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F30" s="52" t="s">
         <v>10</v>
@@ -1754,7 +1754,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="50" t="s">
         <v>54</v>
@@ -1766,7 +1766,7 @@
         <v>8</v>
       </c>
       <c r="E31" s="53" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="F31" s="52" t="s">
         <v>10</v>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" s="50" t="s">
         <v>55</v>
@@ -1789,7 +1789,7 @@
         <v>8</v>
       </c>
       <c r="E32" s="53" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="F32" s="52" t="s">
         <v>10</v>
@@ -1797,12 +1797,12 @@
       <c r="G32" s="52"/>
       <c r="H32" s="52"/>
       <c r="I32" s="52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" s="50" t="s">
         <v>56</v>
@@ -1814,7 +1814,7 @@
         <v>8</v>
       </c>
       <c r="E33" s="53" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="F33" s="52" t="s">
         <v>10</v>
@@ -1822,15 +1822,15 @@
       <c r="G33" s="52"/>
       <c r="H33" s="52"/>
       <c r="I33" s="52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B34" s="50" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="C34" s="51" t="s">
         <v>7</v>
@@ -1839,7 +1839,7 @@
         <v>8</v>
       </c>
       <c r="E34" s="53" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="F34" s="52" t="s">
         <v>10</v>
@@ -1850,10 +1850,10 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" s="51" t="s">
         <v>7</v>
@@ -1873,10 +1873,10 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C36" s="51" t="s">
         <v>7</v>
@@ -1885,7 +1885,7 @@
         <v>8</v>
       </c>
       <c r="E36" s="53" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="F36" s="52" t="s">
         <v>10</v>
@@ -1896,10 +1896,10 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B37" s="50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C37" s="51" t="s">
         <v>7</v>
@@ -1919,10 +1919,10 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B38" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" s="51" t="s">
         <v>7</v>
@@ -1931,7 +1931,7 @@
         <v>8</v>
       </c>
       <c r="E38" s="53" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="F38" s="52" t="s">
         <v>10</v>
@@ -1942,10 +1942,10 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B39" s="50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>7</v>
@@ -1954,7 +1954,7 @@
         <v>8</v>
       </c>
       <c r="E39" s="53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F39" s="52" t="s">
         <v>10</v>
@@ -1965,10 +1965,10 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B40" s="50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C40" s="51" t="s">
         <v>7</v>
@@ -1977,7 +1977,7 @@
         <v>8</v>
       </c>
       <c r="E40" s="53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F40" s="52" t="s">
         <v>10</v>
@@ -1988,10 +1988,10 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B41" s="55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="56" t="s">
         <v>7</v>
@@ -2003,7 +2003,7 @@
         <v>9</v>
       </c>
       <c r="F41" s="57" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G41" s="57"/>
       <c r="H41" s="57"/>
@@ -2011,10 +2011,10 @@
     </row>
     <row r="42" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C42" s="51" t="s">
         <v>7</v>
@@ -2048,7 +2048,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B44" s="65"/>
       <c r="C44" s="65"/>
@@ -2061,10 +2061,10 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="59" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B45" s="60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C45" s="61" t="s">
         <v>7</v>
@@ -2084,10 +2084,10 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B46" s="60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C46" s="61" t="s">
         <v>7</v>
@@ -2107,10 +2107,10 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="59" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B47" s="60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C47" s="61" t="s">
         <v>7</v>
@@ -2130,10 +2130,10 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="59" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B48" s="60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C48" s="61" t="s">
         <v>7</v>
@@ -2153,10 +2153,10 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="59" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B49" s="60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C49" s="61" t="s">
         <v>7</v>
@@ -2176,10 +2176,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B50" s="60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C50" s="61" t="s">
         <v>7</v>
@@ -2188,7 +2188,7 @@
         <v>8</v>
       </c>
       <c r="E50" s="63" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F50" s="62" t="s">
         <v>10</v>

</xml_diff>